<commit_message>
missing mults for hack place, balancing changes
</commit_message>
<xml_diff>
--- a/app/assets/excel/BALANCING.xlsx
+++ b/app/assets/excel/BALANCING.xlsx
@@ -429,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J51"/>
+  <dimension ref="A1:J101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C122" sqref="C122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -574,7 +574,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="4">
-        <f t="shared" ref="B5:B51" si="0">POWER(1.15,A4)*(100*(A4*1.01))</f>
+        <f t="shared" ref="B5:B68" si="0">POWER(1.15,A4)*(100*(A4*1.01))</f>
         <v>460.82512499999984</v>
       </c>
       <c r="C5" s="4"/>
@@ -1101,6 +1101,456 @@
         <v>4663496.2420860706</v>
       </c>
       <c r="C51" s="4"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="3">
+        <v>51</v>
+      </c>
+      <c r="B52" s="4">
+        <f t="shared" si="0"/>
+        <v>5472470.0799989598</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="3">
+        <v>52</v>
+      </c>
+      <c r="B53" s="4">
+        <f t="shared" si="0"/>
+        <v>6419207.4038387798</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="3">
+        <v>53</v>
+      </c>
+      <c r="B54" s="4">
+        <f t="shared" si="0"/>
+        <v>7526835.348030569</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="3">
+        <v>54</v>
+      </c>
+      <c r="B55" s="4">
+        <f t="shared" si="0"/>
+        <v>8822319.5088935215</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="3">
+        <v>55</v>
+      </c>
+      <c r="B56" s="4">
+        <f t="shared" si="0"/>
+        <v>10337095.122684672</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="3">
+        <v>56</v>
+      </c>
+      <c r="B57" s="4">
+        <f t="shared" si="0"/>
+        <v>12107801.231663065</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="3">
+        <v>57</v>
+      </c>
+      <c r="B58" s="4">
+        <f t="shared" si="0"/>
+        <v>14177134.533074569</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="3">
+        <v>58</v>
+      </c>
+      <c r="B59" s="4">
+        <f t="shared" si="0"/>
+        <v>16594842.297197104</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="3">
+        <v>59</v>
+      </c>
+      <c r="B60" s="4">
+        <f t="shared" si="0"/>
+        <v>19418876.863562226</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="3">
+        <v>60</v>
+      </c>
+      <c r="B61" s="4">
+        <f t="shared" si="0"/>
+        <v>22716737.848149944</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="3">
+        <v>61</v>
+      </c>
+      <c r="B62" s="4">
+        <f t="shared" si="0"/>
+        <v>26567032.398683831</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="3">
+        <v>62</v>
+      </c>
+      <c r="B63" s="4">
+        <f t="shared" si="0"/>
+        <v>31061288.712794513</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="3">
+        <v>63</v>
+      </c>
+      <c r="B64" s="4">
+        <f t="shared" si="0"/>
+        <v>36306063.692168012</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="3">
+        <v>64</v>
+      </c>
+      <c r="B65" s="4">
+        <f t="shared" si="0"/>
+        <v>42425392.169315673</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="3">
+        <v>65</v>
+      </c>
+      <c r="B66" s="4">
+        <f t="shared" si="0"/>
+        <v>49563632.756533854</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="3">
+        <v>66</v>
+      </c>
+      <c r="B67" s="4">
+        <f t="shared" si="0"/>
+        <v>57888774.196107909</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="3">
+        <v>67</v>
+      </c>
+      <c r="B68" s="4">
+        <f t="shared" si="0"/>
+        <v>67596276.330532134</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="3">
+        <v>68</v>
+      </c>
+      <c r="B69" s="4">
+        <f t="shared" ref="B69:B101" si="1">POWER(1.15,A68)*(100*(A68*1.01))</f>
+        <v>78913531.685871214</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="3">
+        <v>69</v>
+      </c>
+      <c r="B70" s="4">
+        <f t="shared" si="1"/>
+        <v>92105047.430375069</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="3">
+        <v>70</v>
+      </c>
+      <c r="B71" s="4">
+        <f t="shared" si="1"/>
+        <v>107478463.43529795</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="3">
+        <v>71</v>
+      </c>
+      <c r="B72" s="4">
+        <f t="shared" si="1"/>
+        <v>125391540.67451426</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="3">
+        <v>72</v>
+      </c>
+      <c r="B73" s="4">
+        <f t="shared" si="1"/>
+        <v>146260275.65820125</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="3">
+        <v>73</v>
+      </c>
+      <c r="B74" s="4">
+        <f t="shared" si="1"/>
+        <v>170568321.47181782</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="3">
+        <v>74</v>
+      </c>
+      <c r="B75" s="4">
+        <f t="shared" si="1"/>
+        <v>198877924.82720977</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" s="3">
+        <v>75</v>
+      </c>
+      <c r="B76" s="4">
+        <f t="shared" si="1"/>
+        <v>231842621.95610338</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" s="3">
+        <v>76</v>
+      </c>
+      <c r="B77" s="4">
+        <f t="shared" si="1"/>
+        <v>270221974.91505295</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="3">
+        <v>77</v>
+      </c>
+      <c r="B78" s="4">
+        <f t="shared" si="1"/>
+        <v>314898674.76767504</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="3">
+        <v>78</v>
+      </c>
+      <c r="B79" s="4">
+        <f t="shared" si="1"/>
+        <v>366898390.140495</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="3">
+        <v>79</v>
+      </c>
+      <c r="B80" s="4">
+        <f t="shared" si="1"/>
+        <v>427412799.94288832</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="3">
+        <v>80</v>
+      </c>
+      <c r="B81" s="4">
+        <f t="shared" si="1"/>
+        <v>497826318.90783852</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="3">
+        <v>81</v>
+      </c>
+      <c r="B82" s="4">
+        <f t="shared" si="1"/>
+        <v>579747105.56355858</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="3">
+        <v>82</v>
+      </c>
+      <c r="B83" s="4">
+        <f t="shared" si="1"/>
+        <v>675043036.04056835</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="3">
+        <v>83</v>
+      </c>
+      <c r="B84" s="4">
+        <f t="shared" si="1"/>
+        <v>785883435.78550112</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="3">
+        <v>84</v>
+      </c>
+      <c r="B85" s="4">
+        <f t="shared" si="1"/>
+        <v>914787487.14300096</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="3">
+        <v>85</v>
+      </c>
+      <c r="B86" s="4">
+        <f t="shared" si="1"/>
+        <v>1064680376.602577</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87" s="3">
+        <v>86</v>
+      </c>
+      <c r="B87" s="4">
+        <f t="shared" si="1"/>
+        <v>1238958414.4393082</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88" s="3">
+        <v>87</v>
+      </c>
+      <c r="B88" s="4">
+        <f t="shared" si="1"/>
+        <v>1441564555.153501</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89" s="3">
+        <v>88</v>
+      </c>
+      <c r="B89" s="4">
+        <f t="shared" si="1"/>
+        <v>1677075973.757067</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90" s="3">
+        <v>89</v>
+      </c>
+      <c r="B90" s="4">
+        <f t="shared" si="1"/>
+        <v>1950805615.4507487</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91" s="3">
+        <v>90</v>
+      </c>
+      <c r="B91" s="4">
+        <f t="shared" si="1"/>
+        <v>2268919940.2430015</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92" s="3">
+        <v>91</v>
+      </c>
+      <c r="B92" s="4">
+        <f t="shared" si="1"/>
+        <v>2638575436.1252885</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93" s="3">
+        <v>92</v>
+      </c>
+      <c r="B93" s="4">
+        <f t="shared" si="1"/>
+        <v>3068076882.1167932</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94" s="3">
+        <v>93</v>
+      </c>
+      <c r="B94" s="4">
+        <f t="shared" si="1"/>
+        <v>3567060814.5929303</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95" s="3">
+        <v>94</v>
+      </c>
+      <c r="B95" s="4">
+        <f t="shared" si="1"/>
+        <v>4146708196.9642816</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96" s="3">
+        <v>95</v>
+      </c>
+      <c r="B96" s="4">
+        <f t="shared" si="1"/>
+        <v>4819990925.7186975</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97" s="3">
+        <v>96</v>
+      </c>
+      <c r="B97" s="4">
+        <f t="shared" si="1"/>
+        <v>5601957538.6677399</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98" s="3">
+        <v>97</v>
+      </c>
+      <c r="B98" s="4">
+        <f t="shared" si="1"/>
+        <v>6510064339.6728239</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99" s="3">
+        <v>98</v>
+      </c>
+      <c r="B99" s="4">
+        <f t="shared" si="1"/>
+        <v>7564559136.3594112</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100" s="3">
+        <v>99</v>
+      </c>
+      <c r="B100" s="4">
+        <f t="shared" si="1"/>
+        <v>8788925924.409338</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101" s="3">
+        <v>100</v>
+      </c>
+      <c r="B101" s="4">
+        <f t="shared" si="1"/>
+        <v>10210400168.30615</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>